<commit_message>
adding years to excel
</commit_message>
<xml_diff>
--- a/excel_files/top_grossing_by_year.xlsx
+++ b/excel_files/top_grossing_by_year.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilychristiansen/Documents/97emilylc.github.io/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE24823-CE69-2747-85B0-D6C2EEEA69E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F58B23-E34C-8C4A-AC4A-117BFBD9DF1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16720" firstSheet="12" activeTab="23" xr2:uid="{9023697C-5DAC-8D4B-B865-EBFD92B0B869}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16720" firstSheet="19" activeTab="25" xr2:uid="{9023697C-5DAC-8D4B-B865-EBFD92B0B869}"/>
   </bookViews>
   <sheets>
     <sheet name="1980" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,9 @@
     <sheet name="2000" sheetId="21" r:id="rId21"/>
     <sheet name="2001" sheetId="22" r:id="rId22"/>
     <sheet name="2002" sheetId="23" r:id="rId23"/>
-    <sheet name="Sheet24" sheetId="24" r:id="rId24"/>
+    <sheet name="2003" sheetId="24" r:id="rId24"/>
+    <sheet name="2004" sheetId="25" r:id="rId25"/>
+    <sheet name="Sheet2" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -54,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2404" uniqueCount="2404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2504" uniqueCount="2503">
   <si>
     <t>The Empire Strikes Back</t>
   </si>
@@ -7266,6 +7268,303 @@
   </si>
   <si>
     <t>Dumb and Dumberer: When Harry Met Lloyd</t>
+  </si>
+  <si>
+    <t>Shrek 2</t>
+  </si>
+  <si>
+    <t>Spider-Man 2</t>
+  </si>
+  <si>
+    <t>The Passion of the Christ</t>
+  </si>
+  <si>
+    <t>Meet the Fockers</t>
+  </si>
+  <si>
+    <t>The Incredibles</t>
+  </si>
+  <si>
+    <t>Harry Potter and the Prisoner of Azkaban</t>
+  </si>
+  <si>
+    <t>The Day After Tomorrow</t>
+  </si>
+  <si>
+    <t>The Bourne Supremacy</t>
+  </si>
+  <si>
+    <t>National Treasure</t>
+  </si>
+  <si>
+    <t>The Polar Express</t>
+  </si>
+  <si>
+    <t>Shark Tale</t>
+  </si>
+  <si>
+    <t>I, Robot</t>
+  </si>
+  <si>
+    <t>Troy</t>
+  </si>
+  <si>
+    <t>Ocean's Twelve</t>
+  </si>
+  <si>
+    <t>50 First Dates</t>
+  </si>
+  <si>
+    <t>Van Helsing</t>
+  </si>
+  <si>
+    <t>Fahrenheit 9/11</t>
+  </si>
+  <si>
+    <t>Lemony Snicket's A Series of Unfortunate Events</t>
+  </si>
+  <si>
+    <t>DodgeBall: A True Underdog Story</t>
+  </si>
+  <si>
+    <t>The Village</t>
+  </si>
+  <si>
+    <t>The Grudge</t>
+  </si>
+  <si>
+    <t>The Aviator</t>
+  </si>
+  <si>
+    <t>Collateral</t>
+  </si>
+  <si>
+    <t>Million Dollar Baby</t>
+  </si>
+  <si>
+    <t>The Princess Diaries 2: Royal Engagement</t>
+  </si>
+  <si>
+    <t>Starsky and Hutch</t>
+  </si>
+  <si>
+    <t>Along Came Polly</t>
+  </si>
+  <si>
+    <t>Mean Girls</t>
+  </si>
+  <si>
+    <t>The SpongeBob SquarePants Movie</t>
+  </si>
+  <si>
+    <t>Anchorman: The Legend of Ron Burgundy</t>
+  </si>
+  <si>
+    <t>Scooby-Doo 2: Monsters Unleashed</t>
+  </si>
+  <si>
+    <t>The Notebook</t>
+  </si>
+  <si>
+    <t>Alien Vs. Predator</t>
+  </si>
+  <si>
+    <t>Man on Fire</t>
+  </si>
+  <si>
+    <t>The Terminal</t>
+  </si>
+  <si>
+    <t>Garfield: The Movie</t>
+  </si>
+  <si>
+    <t>Ray</t>
+  </si>
+  <si>
+    <t>Ladder 49</t>
+  </si>
+  <si>
+    <t>Christmas with the Kranks</t>
+  </si>
+  <si>
+    <t>Sideways</t>
+  </si>
+  <si>
+    <t>White Chicks</t>
+  </si>
+  <si>
+    <t>Hidalgo</t>
+  </si>
+  <si>
+    <t>The Forgotten</t>
+  </si>
+  <si>
+    <t>Kill Bill Vol. 2</t>
+  </si>
+  <si>
+    <t>The Manchurian Candidate</t>
+  </si>
+  <si>
+    <t>Barbershop 2: Back in Business</t>
+  </si>
+  <si>
+    <t>Miracle</t>
+  </si>
+  <si>
+    <t>Friday Night Lights</t>
+  </si>
+  <si>
+    <t>Hellboy</t>
+  </si>
+  <si>
+    <t>The Stepford Wives</t>
+  </si>
+  <si>
+    <t>Dawn of the Dead</t>
+  </si>
+  <si>
+    <t>Without a Paddle</t>
+  </si>
+  <si>
+    <t>The Butterfly Effect</t>
+  </si>
+  <si>
+    <t>Shall We Dance</t>
+  </si>
+  <si>
+    <t>The Chronicles of Riddick</t>
+  </si>
+  <si>
+    <t>13 Going on 30</t>
+  </si>
+  <si>
+    <t>Saw</t>
+  </si>
+  <si>
+    <t>Blade: Trinity</t>
+  </si>
+  <si>
+    <t>King Arthur</t>
+  </si>
+  <si>
+    <t>Finding Neverland</t>
+  </si>
+  <si>
+    <t>A Cinderella Story</t>
+  </si>
+  <si>
+    <t>The Phantom of the Opera</t>
+  </si>
+  <si>
+    <t>Resident Evil: Apocalypse</t>
+  </si>
+  <si>
+    <t>Home on the Range</t>
+  </si>
+  <si>
+    <t>Fat Albert</t>
+  </si>
+  <si>
+    <t>Secret Window</t>
+  </si>
+  <si>
+    <t>Walking Tall</t>
+  </si>
+  <si>
+    <t>In Good Company</t>
+  </si>
+  <si>
+    <t>Napoleon Dynamite</t>
+  </si>
+  <si>
+    <t>Spanglish</t>
+  </si>
+  <si>
+    <t>Exorcist: The Beginning</t>
+  </si>
+  <si>
+    <t>You Got Served</t>
+  </si>
+  <si>
+    <t>Bridget Jones: The Edge of Reason</t>
+  </si>
+  <si>
+    <t>Catwoman</t>
+  </si>
+  <si>
+    <t>The Ladykillers</t>
+  </si>
+  <si>
+    <t>Sky Captain and the World of Tomorrow</t>
+  </si>
+  <si>
+    <t>Raising Helen</t>
+  </si>
+  <si>
+    <t>Taxi</t>
+  </si>
+  <si>
+    <t>Eternal Sunshine of the Spotless Mind</t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>Closer</t>
+  </si>
+  <si>
+    <t>The Punisher</t>
+  </si>
+  <si>
+    <t>Team America: World Police</t>
+  </si>
+  <si>
+    <t>Taking Lives</t>
+  </si>
+  <si>
+    <t>Anacondas: The Hunt for the Blood Orchid</t>
+  </si>
+  <si>
+    <t>Cellular</t>
+  </si>
+  <si>
+    <t>Johnson Family Vacation</t>
+  </si>
+  <si>
+    <t>Open Water</t>
+  </si>
+  <si>
+    <t>Confessions of a Teenage Drama Queen</t>
+  </si>
+  <si>
+    <t>After the Sunset</t>
+  </si>
+  <si>
+    <t>The Prince and Me</t>
+  </si>
+  <si>
+    <t>Garden State</t>
+  </si>
+  <si>
+    <t>Jersey Girl</t>
+  </si>
+  <si>
+    <t>Twisted</t>
+  </si>
+  <si>
+    <t>The Life Aquatic with Steve Zissou</t>
+  </si>
+  <si>
+    <t>Around the World in 80 Days</t>
+  </si>
+  <si>
+    <t>Agent Cody Banks 2: Destination London</t>
+  </si>
+  <si>
+    <t>Hotel Rwanda</t>
+  </si>
+  <si>
+    <t>Ella Enchanted</t>
   </si>
 </sst>
 </file>
@@ -29378,7 +29677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCB130F-3CF9-CF48-A27C-7F18753162FC}">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -30885,6 +31184,1531 @@
       <c r="I100" s="13"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A11FAB7-9BEC-B24D-93BA-FAA2D106EDA6}">
+  <dimension ref="A1:I100"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="41.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="4">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>2404</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>2405</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>2406</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="13"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>2407</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>5</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>2408</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>2409</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="13"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>2410</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="13"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>8</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>2411</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>9</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>2412</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>10</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>2413</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="13"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>11</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>2414</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="13"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>2415</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="13"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>13</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>2416</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="13"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>14</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>2417</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="13"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>15</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>2418</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="13"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>16</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>2419</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="13"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>17</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>2420</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="13"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>18</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>2421</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="13"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>19</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>2422</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>20</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>2423</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="13"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>21</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>2424</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="13"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>22</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>2425</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="13"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>23</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>2426</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="13"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>24</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>2427</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="13"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>25</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>2428</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="13"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>26</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>2429</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="13"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
+        <v>27</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>2430</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="13"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <v>28</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>2431</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="13"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>29</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>2432</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="13"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>30</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>2433</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="13"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
+        <v>31</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>2434</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="13"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
+        <v>32</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>2435</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="13"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="4">
+        <v>33</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>2436</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="13"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
+        <v>34</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>2437</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="13"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="4">
+        <v>35</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>2438</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="13"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
+        <v>36</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>2439</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="13"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="4">
+        <v>37</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>2440</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="13"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="4">
+        <v>38</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>2441</v>
+      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="13"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="4">
+        <v>39</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>2442</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="13"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
+        <v>40</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>2443</v>
+      </c>
+      <c r="C40" s="4"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="13"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="4">
+        <v>41</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>2444</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="13"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="4">
+        <v>42</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>2445</v>
+      </c>
+      <c r="C42" s="4"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="13"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="4">
+        <v>43</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>2446</v>
+      </c>
+      <c r="C43" s="4"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="13"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="4">
+        <v>44</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>2447</v>
+      </c>
+      <c r="C44" s="4"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="13"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="4">
+        <v>45</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>2448</v>
+      </c>
+      <c r="C45" s="4"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="13"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="4">
+        <v>46</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>2449</v>
+      </c>
+      <c r="C46" s="4"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="13"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="4">
+        <v>47</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>2450</v>
+      </c>
+      <c r="C47" s="4"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="13"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="4">
+        <v>48</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>2451</v>
+      </c>
+      <c r="C48" s="4"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="13"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="4">
+        <v>49</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>2452</v>
+      </c>
+      <c r="C49" s="4"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="13"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="4">
+        <v>50</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>2453</v>
+      </c>
+      <c r="C50" s="4"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="13"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="4">
+        <v>51</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>2454</v>
+      </c>
+      <c r="C51" s="4"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="13"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="4">
+        <v>52</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>2455</v>
+      </c>
+      <c r="C52" s="4"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="13"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="4">
+        <v>53</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>2456</v>
+      </c>
+      <c r="C53" s="4"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="13"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="4">
+        <v>54</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>2457</v>
+      </c>
+      <c r="C54" s="4"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="13"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="4">
+        <v>55</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>2458</v>
+      </c>
+      <c r="C55" s="4"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="13"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="4">
+        <v>56</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>2459</v>
+      </c>
+      <c r="C56" s="4"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="13"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="4">
+        <v>57</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>2460</v>
+      </c>
+      <c r="C57" s="4"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="13"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="4">
+        <v>58</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C58" s="4"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="13"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="4">
+        <v>59</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>2461</v>
+      </c>
+      <c r="C59" s="4"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="13"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="4">
+        <v>60</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>2462</v>
+      </c>
+      <c r="C60" s="4"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="13"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="4">
+        <v>61</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>2463</v>
+      </c>
+      <c r="C61" s="4"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="13"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="4">
+        <v>62</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>2464</v>
+      </c>
+      <c r="C62" s="4"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="13"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="4">
+        <v>63</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>2465</v>
+      </c>
+      <c r="C63" s="4"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="13"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="4">
+        <v>64</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>2466</v>
+      </c>
+      <c r="C64" s="4"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="13"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="4">
+        <v>65</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>2467</v>
+      </c>
+      <c r="C65" s="4"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="13"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="4">
+        <v>66</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>2468</v>
+      </c>
+      <c r="C66" s="4"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="13"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="4">
+        <v>67</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>2469</v>
+      </c>
+      <c r="C67" s="4"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="13"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="4">
+        <v>68</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C68" s="4"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="13"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="4">
+        <v>69</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>2471</v>
+      </c>
+      <c r="C69" s="4"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="4"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="13"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="4">
+        <v>70</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>2472</v>
+      </c>
+      <c r="C70" s="4"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="4"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="13"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" s="4">
+        <v>71</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>2473</v>
+      </c>
+      <c r="C71" s="4"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="13"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" s="4">
+        <v>72</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>2474</v>
+      </c>
+      <c r="C72" s="4"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="13"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" s="4">
+        <v>73</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>2475</v>
+      </c>
+      <c r="C73" s="4"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="13"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" s="4">
+        <v>74</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>2476</v>
+      </c>
+      <c r="C74" s="4"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="13"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" s="4">
+        <v>75</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>2477</v>
+      </c>
+      <c r="C75" s="4"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="13"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76" s="4">
+        <v>76</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>2478</v>
+      </c>
+      <c r="C76" s="4"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="13"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A77" s="4">
+        <v>77</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>2479</v>
+      </c>
+      <c r="C77" s="4"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="5"/>
+      <c r="I77" s="13"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A78" s="4">
+        <v>78</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>2480</v>
+      </c>
+      <c r="C78" s="4"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="13"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A79" s="4">
+        <v>79</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>2481</v>
+      </c>
+      <c r="C79" s="4"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="13"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80" s="4">
+        <v>80</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>2482</v>
+      </c>
+      <c r="C80" s="4"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="5"/>
+      <c r="I80" s="13"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" s="4">
+        <v>81</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>2483</v>
+      </c>
+      <c r="C81" s="4"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="5"/>
+      <c r="I81" s="13"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" s="4">
+        <v>82</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>2484</v>
+      </c>
+      <c r="C82" s="4"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="4"/>
+      <c r="H82" s="5"/>
+      <c r="I82" s="13"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83" s="4">
+        <v>83</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>2485</v>
+      </c>
+      <c r="C83" s="4"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="5"/>
+      <c r="I83" s="13"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" s="4">
+        <v>84</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>2486</v>
+      </c>
+      <c r="C84" s="4"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="2"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="13"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" s="4">
+        <v>85</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>2487</v>
+      </c>
+      <c r="C85" s="4"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="5"/>
+      <c r="I85" s="13"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" s="4">
+        <v>86</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>2488</v>
+      </c>
+      <c r="C86" s="4"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="5"/>
+      <c r="I86" s="13"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" s="4">
+        <v>87</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>2489</v>
+      </c>
+      <c r="C87" s="4"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="5"/>
+      <c r="I87" s="13"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" s="4">
+        <v>88</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>2490</v>
+      </c>
+      <c r="C88" s="4"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="2"/>
+      <c r="H88" s="5"/>
+      <c r="I88" s="13"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" s="4">
+        <v>89</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>2491</v>
+      </c>
+      <c r="C89" s="4"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="5"/>
+      <c r="I89" s="13"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" s="4">
+        <v>90</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>2492</v>
+      </c>
+      <c r="C90" s="4"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="2"/>
+      <c r="H90" s="5"/>
+      <c r="I90" s="13"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" s="4">
+        <v>91</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>2493</v>
+      </c>
+      <c r="C91" s="4"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="5"/>
+      <c r="I91" s="13"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92" s="4">
+        <v>92</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>2494</v>
+      </c>
+      <c r="C92" s="4"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="5"/>
+      <c r="I92" s="13"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" s="4">
+        <v>93</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>2495</v>
+      </c>
+      <c r="C93" s="4"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="5"/>
+      <c r="I93" s="13"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" s="4">
+        <v>94</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>2496</v>
+      </c>
+      <c r="C94" s="4"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="2"/>
+      <c r="H94" s="5"/>
+      <c r="I94" s="13"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95" s="4">
+        <v>95</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>2497</v>
+      </c>
+      <c r="C95" s="4"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="2"/>
+      <c r="H95" s="5"/>
+      <c r="I95" s="13"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" s="4">
+        <v>96</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>2498</v>
+      </c>
+      <c r="C96" s="4"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="4"/>
+      <c r="H96" s="5"/>
+      <c r="I96" s="13"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" s="4">
+        <v>97</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>2499</v>
+      </c>
+      <c r="C97" s="4"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="2"/>
+      <c r="H97" s="5"/>
+      <c r="I97" s="13"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" s="4">
+        <v>98</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>2500</v>
+      </c>
+      <c r="C98" s="4"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="3"/>
+      <c r="G98" s="2"/>
+      <c r="H98" s="5"/>
+      <c r="I98" s="13"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" s="4">
+        <v>99</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>2501</v>
+      </c>
+      <c r="C99" s="4"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="3"/>
+      <c r="G99" s="4"/>
+      <c r="H99" s="5"/>
+      <c r="I99" s="13"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A100" s="4">
+        <v>100</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>2502</v>
+      </c>
+      <c r="C100" s="4"/>
+      <c r="D100" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91C04118-16EF-9141-9F73-E3D68BD193E7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
half way throiugh 1981
</commit_message>
<xml_diff>
--- a/excel_files/top_grossing_by_year.xlsx
+++ b/excel_files/top_grossing_by_year.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilychristiansen/Documents/97emilylc.github.io/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC3BB74-6DF4-0545-BFC7-770D41CED008}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE96791-447E-834F-83D9-8A55845C5EDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16720" xr2:uid="{9023697C-5DAC-8D4B-B865-EBFD92B0B869}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16720" activeTab="1" xr2:uid="{9023697C-5DAC-8D4B-B865-EBFD92B0B869}"/>
   </bookViews>
   <sheets>
     <sheet name="1980" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3974" uniqueCount="3946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4043" uniqueCount="3978">
   <si>
     <t>The Empire Strikes Back</t>
   </si>
@@ -11907,6 +11907,102 @@
   </si>
   <si>
     <t>England</t>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>Culver City, CA</t>
+  </si>
+  <si>
+    <t>Pasadena, CA</t>
+  </si>
+  <si>
+    <t>Staten Island, NY</t>
+  </si>
+  <si>
+    <t>New York State</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Travelling</t>
+  </si>
+  <si>
+    <t>South Bronx</t>
+  </si>
+  <si>
+    <t>Long Island, NY</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Buffalo NY</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
+  </si>
+  <si>
+    <t>Acapulco</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>New Hampshire</t>
+  </si>
+  <si>
+    <t>Louisville</t>
+  </si>
+  <si>
+    <t>Connecticut to California</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>greece</t>
+  </si>
+  <si>
+    <t>miami</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>West Point, New York</t>
+  </si>
+  <si>
+    <t>The Bronx, NY</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Lyme Regis</t>
+  </si>
+  <si>
+    <t>alburquerque</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>New England</t>
+  </si>
+  <si>
+    <t>Yorkshire</t>
   </si>
 </sst>
 </file>
@@ -12387,8 +12483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C56C22-15EA-6D4C-952A-C51C8596E6F0}">
   <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13213,6 +13309,12 @@
       <c r="B74" s="6" t="s">
         <v>73</v>
       </c>
+      <c r="C74" t="s">
+        <v>3936</v>
+      </c>
+      <c r="D74" t="s">
+        <v>3928</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
@@ -13221,6 +13323,9 @@
       <c r="B75" s="6" t="s">
         <v>74</v>
       </c>
+      <c r="C75" t="s">
+        <v>3906</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
@@ -13229,6 +13334,9 @@
       <c r="B76" s="6" t="s">
         <v>75</v>
       </c>
+      <c r="C76" t="s">
+        <v>3935</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
@@ -13237,6 +13345,9 @@
       <c r="B77" s="6" t="s">
         <v>76</v>
       </c>
+      <c r="C77" t="s">
+        <v>3946</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
@@ -13245,6 +13356,9 @@
       <c r="B78" s="6" t="s">
         <v>77</v>
       </c>
+      <c r="C78" t="s">
+        <v>3947</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
@@ -13253,6 +13367,9 @@
       <c r="B79" s="6" t="s">
         <v>78</v>
       </c>
+      <c r="C79" t="s">
+        <v>3946</v>
+      </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
@@ -13261,165 +13378,231 @@
       <c r="B80" s="6" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C80" t="s">
+        <v>3915</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
         <v>81</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C81" t="s">
+        <v>3948</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
         <v>82</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C82" t="s">
+        <v>3907</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
         <v>83</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C83" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>84</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C84" t="s">
+        <v>3950</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>85</v>
       </c>
       <c r="B85" s="6" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C85" t="s">
+        <v>3912</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>86</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C86" t="s">
+        <v>3951</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
         <v>87</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C87" t="s">
+        <v>3952</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
         <v>88</v>
       </c>
       <c r="B88" s="6" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C88" t="s">
+        <v>3953</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
         <v>89</v>
       </c>
       <c r="B89" s="6" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C89" t="s">
+        <v>3954</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
         <v>90</v>
       </c>
       <c r="B90" s="6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C90" t="s">
+        <v>3955</v>
+      </c>
+      <c r="D90" t="s">
+        <v>3921</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
         <v>91</v>
       </c>
       <c r="B91" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C91" t="s">
+        <v>3956</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
         <v>92</v>
       </c>
       <c r="B92" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C92" t="s">
+        <v>3957</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="4">
         <v>93</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C93" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="4">
         <v>94</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C94" t="s">
+        <v>3939</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="4">
         <v>95</v>
       </c>
       <c r="B95" s="6" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C95" t="s">
+        <v>3959</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="4">
         <v>96</v>
       </c>
       <c r="B96" s="6" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C96" t="s">
+        <v>3939</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="4">
         <v>97</v>
       </c>
       <c r="B97" s="6" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C97" t="s">
+        <v>3906</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="4">
         <v>98</v>
       </c>
       <c r="B98" s="6" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C98" t="s">
+        <v>3960</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="4">
         <v>99</v>
       </c>
       <c r="B99" s="6" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C99" t="s">
+        <v>3961</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="4">
         <v>100</v>
       </c>
       <c r="B100" s="6" t="s">
         <v>99</v>
+      </c>
+      <c r="C100" t="s">
+        <v>3906</v>
       </c>
     </row>
   </sheetData>
@@ -27056,8 +27239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A318C304-65A2-6040-9278-5112EAD65301}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27072,7 +27255,9 @@
       <c r="B1" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="C1" s="4" t="s">
+        <v>3936</v>
+      </c>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="3"/>
@@ -27086,7 +27271,9 @@
       <c r="B2" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>3962</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="2"/>
       <c r="F2" s="3"/>
@@ -27100,7 +27287,9 @@
       <c r="B3" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>3917</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
@@ -27114,7 +27303,9 @@
       <c r="B4" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>3917</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="4"/>
       <c r="F4" s="3"/>
@@ -27128,7 +27319,9 @@
       <c r="B5" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>3963</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="4"/>
       <c r="F5" s="3"/>
@@ -27142,7 +27335,9 @@
       <c r="B6" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>3964</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="2"/>
       <c r="F6" s="3"/>
@@ -27156,8 +27351,12 @@
       <c r="B7" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="1"/>
+      <c r="C7" s="4" t="s">
+        <v>3915</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>3928</v>
+      </c>
       <c r="E7" s="4"/>
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
@@ -27170,7 +27369,9 @@
       <c r="B8" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>3965</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="4"/>
       <c r="F8" s="3"/>
@@ -27184,7 +27385,9 @@
       <c r="B9" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>3917</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="4"/>
       <c r="F9" s="3"/>
@@ -27198,7 +27401,9 @@
       <c r="B10" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>3961</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="4"/>
       <c r="F10" s="3"/>
@@ -27212,8 +27417,12 @@
       <c r="B11" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="4" t="s">
+        <v>3966</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>3928</v>
+      </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -27226,7 +27435,9 @@
       <c r="B12" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>3967</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="E12" s="4"/>
       <c r="F12" s="3"/>
@@ -27240,7 +27451,9 @@
       <c r="B13" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>3950</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="4"/>
       <c r="F13" s="3"/>
@@ -27254,7 +27467,9 @@
       <c r="B14" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>3961</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -27268,7 +27483,9 @@
       <c r="B15" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>3968</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -27282,7 +27499,9 @@
       <c r="B16" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>3969</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="4"/>
       <c r="F16" s="3"/>
@@ -27296,7 +27515,9 @@
       <c r="B17" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>3911</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
       <c r="F17" s="3"/>
@@ -27310,8 +27531,12 @@
       <c r="B18" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="1"/>
+      <c r="C18" s="4" t="s">
+        <v>3945</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>3928</v>
+      </c>
       <c r="E18" s="4"/>
       <c r="F18" s="3"/>
       <c r="G18" s="4"/>
@@ -27324,7 +27549,9 @@
       <c r="B19" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>3961</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="4"/>
       <c r="F19" s="3"/>
@@ -27338,7 +27565,9 @@
       <c r="B20" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="C20" s="4" t="s">
+        <v>1315</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="4"/>
       <c r="F20" s="3"/>
@@ -27352,7 +27581,9 @@
       <c r="B21" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>3915</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="4"/>
       <c r="F21" s="3"/>
@@ -27366,7 +27597,9 @@
       <c r="B22" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="4" t="s">
+        <v>2213</v>
+      </c>
       <c r="D22" s="1"/>
       <c r="E22" s="4"/>
       <c r="F22" s="3"/>
@@ -27380,7 +27613,9 @@
       <c r="B23" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>3915</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="4"/>
       <c r="F23" s="3"/>
@@ -27394,7 +27629,9 @@
       <c r="B24" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C24" s="4"/>
+      <c r="C24" s="4" t="s">
+        <v>3961</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
       <c r="F24" s="3"/>
@@ -27408,7 +27645,9 @@
       <c r="B25" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C25" s="4"/>
+      <c r="C25" s="4" t="s">
+        <v>3970</v>
+      </c>
       <c r="D25" s="1"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -27422,7 +27661,9 @@
       <c r="B26" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C26" s="4"/>
+      <c r="C26" s="4" t="s">
+        <v>3971</v>
+      </c>
       <c r="D26" s="1"/>
       <c r="E26" s="4"/>
       <c r="F26" s="3"/>
@@ -27436,8 +27677,12 @@
       <c r="B27" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="1"/>
+      <c r="C27" s="4" t="s">
+        <v>3972</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>3928</v>
+      </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
@@ -27450,7 +27695,9 @@
       <c r="B28" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>3973</v>
+      </c>
       <c r="D28" s="1"/>
       <c r="E28" s="4"/>
       <c r="F28" s="3"/>
@@ -27464,7 +27711,9 @@
       <c r="B29" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C29" s="4"/>
+      <c r="C29" s="4" t="s">
+        <v>3917</v>
+      </c>
       <c r="D29" s="1"/>
       <c r="E29" s="2"/>
       <c r="F29" s="4"/>
@@ -27478,7 +27727,9 @@
       <c r="B30" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C30" s="4"/>
+      <c r="C30" s="4" t="s">
+        <v>3974</v>
+      </c>
       <c r="D30" s="1"/>
       <c r="E30" s="4"/>
       <c r="F30" s="3"/>
@@ -27492,7 +27743,9 @@
       <c r="B31" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C31" s="4"/>
+      <c r="C31" s="4" t="s">
+        <v>3912</v>
+      </c>
       <c r="D31" s="1"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -27506,7 +27759,9 @@
       <c r="B32" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C32" s="4"/>
+      <c r="C32" s="4" t="s">
+        <v>3912</v>
+      </c>
       <c r="D32" s="1"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -27520,7 +27775,9 @@
       <c r="B33" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C33" s="4"/>
+      <c r="C33" s="4" t="s">
+        <v>3975</v>
+      </c>
       <c r="D33" s="1"/>
       <c r="E33" s="4"/>
       <c r="F33" s="3"/>
@@ -27534,7 +27791,9 @@
       <c r="B34" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="C34" s="4"/>
+      <c r="C34" s="4" t="s">
+        <v>3976</v>
+      </c>
       <c r="D34" s="1"/>
       <c r="E34" s="4"/>
       <c r="F34" s="3"/>
@@ -27548,7 +27807,9 @@
       <c r="B35" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C35" s="4"/>
+      <c r="C35" s="4" t="s">
+        <v>3940</v>
+      </c>
       <c r="D35" s="1"/>
       <c r="E35" s="4"/>
       <c r="F35" s="3"/>
@@ -27562,7 +27823,9 @@
       <c r="B36" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C36" s="4"/>
+      <c r="C36" s="4" t="s">
+        <v>3977</v>
+      </c>
       <c r="D36" s="1"/>
       <c r="E36" s="4"/>
       <c r="F36" s="3"/>

</xml_diff>

<commit_message>
starting now at 2018
</commit_message>
<xml_diff>
--- a/excel_files/top_grossing_by_year.xlsx
+++ b/excel_files/top_grossing_by_year.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilychristiansen/Documents/97emilylc.github.io/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FA0122-4212-8043-BD28-00CDCD195FD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD527B6-F31F-6743-8DAD-6BFE17F9A340}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16720" firstSheet="24" activeTab="38" xr2:uid="{9023697C-5DAC-8D4B-B865-EBFD92B0B869}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="13960" windowHeight="17540" firstSheet="24" activeTab="38" xr2:uid="{9023697C-5DAC-8D4B-B865-EBFD92B0B869}"/>
   </bookViews>
   <sheets>
     <sheet name="1980" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4043" uniqueCount="3978">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4070" uniqueCount="3985">
   <si>
     <t>The Empire Strikes Back</t>
   </si>
@@ -12004,6 +12004,27 @@
   </si>
   <si>
     <t>Yorkshire</t>
+  </si>
+  <si>
+    <t>Tanzania, Africa</t>
+  </si>
+  <si>
+    <t>Fictional</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>San Fransisco</t>
+  </si>
+  <si>
+    <t>New Paltz, New York</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Romania</t>
   </si>
 </sst>
 </file>
@@ -58674,8 +58695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED12B06-54D1-D244-9F50-D6160AB448D7}">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -58690,7 +58711,9 @@
       <c r="B1" s="6" t="s">
         <v>3795</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="C1" s="4" t="s">
+        <v>3978</v>
+      </c>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="3"/>
@@ -58705,7 +58728,9 @@
       <c r="B2" s="6" t="s">
         <v>3796</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>3894</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="2"/>
       <c r="F2" s="3"/>
@@ -58720,7 +58745,9 @@
       <c r="B3" s="6" t="s">
         <v>3797</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>3979</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
@@ -58735,7 +58762,9 @@
       <c r="B4" s="6" t="s">
         <v>3798</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>3980</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
@@ -58750,7 +58779,9 @@
       <c r="B5" s="6" t="s">
         <v>3799</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>3939</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="2"/>
       <c r="F5" s="3"/>
@@ -58765,7 +58796,9 @@
       <c r="B6" s="6" t="s">
         <v>3800</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>3917</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="2"/>
       <c r="F6" s="3"/>
@@ -58780,7 +58813,9 @@
       <c r="B7" s="6" t="s">
         <v>3801</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>3979</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="2"/>
       <c r="F7" s="3"/>
@@ -58795,7 +58830,9 @@
       <c r="B8" s="6" t="s">
         <v>3802</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>3915</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="2"/>
       <c r="F8" s="3"/>
@@ -58810,7 +58847,9 @@
       <c r="B9" s="6" t="s">
         <v>3803</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>3981</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="2"/>
       <c r="F9" s="3"/>
@@ -58825,7 +58864,9 @@
       <c r="B10" s="6" t="s">
         <v>3804</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>3915</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="2"/>
       <c r="F10" s="3"/>
@@ -58840,7 +58881,9 @@
       <c r="B11" s="6" t="s">
         <v>3805</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>3906</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
       <c r="F11" s="3"/>
@@ -58855,7 +58898,9 @@
       <c r="B12" s="6" t="s">
         <v>3806</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>3894</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
       <c r="F12" s="3"/>
@@ -58870,7 +58915,9 @@
       <c r="B13" s="6" t="s">
         <v>3807</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>3981</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
       <c r="F13" s="3"/>
@@ -58885,7 +58932,9 @@
       <c r="B14" s="6" t="s">
         <v>3808</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>3979</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
       <c r="F14" s="3"/>
@@ -58900,7 +58949,9 @@
       <c r="B15" s="6" t="s">
         <v>3809</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>3565</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
       <c r="F15" s="3"/>
@@ -58915,7 +58966,9 @@
       <c r="B16" s="6" t="s">
         <v>3810</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>3982</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
       <c r="F16" s="3"/>
@@ -58930,7 +58983,9 @@
       <c r="B17" s="6" t="s">
         <v>3811</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>3983</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
       <c r="F17" s="3"/>
@@ -58945,7 +59000,9 @@
       <c r="B18" s="6" t="s">
         <v>3812</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>3915</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
       <c r="F18" s="3"/>
@@ -58960,7 +59017,9 @@
       <c r="B19" s="6" t="s">
         <v>3813</v>
       </c>
-      <c r="C19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>3984</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
       <c r="F19" s="3"/>
@@ -58975,8 +59034,12 @@
       <c r="B20" s="6" t="s">
         <v>3814</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="1"/>
+      <c r="C20" s="4" t="s">
+        <v>3915</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>3921</v>
+      </c>
       <c r="E20" s="2"/>
       <c r="F20" s="3"/>
       <c r="G20" s="2"/>
@@ -58990,7 +59053,9 @@
       <c r="B21" s="6" t="s">
         <v>3815</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>3974</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
       <c r="F21" s="3"/>
@@ -59005,7 +59070,9 @@
       <c r="B22" s="6" t="s">
         <v>3816</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="4" t="s">
+        <v>3939</v>
+      </c>
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
       <c r="F22" s="3"/>
@@ -59020,7 +59087,9 @@
       <c r="B23" s="6" t="s">
         <v>3817</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>3912</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
       <c r="F23" s="3"/>
@@ -59035,7 +59104,9 @@
       <c r="B24" s="6" t="s">
         <v>3818</v>
       </c>
-      <c r="C24" s="4"/>
+      <c r="C24" s="4" t="s">
+        <v>3979</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
       <c r="F24" s="3"/>
@@ -59050,7 +59121,9 @@
       <c r="B25" s="6" t="s">
         <v>3819</v>
       </c>
-      <c r="C25" s="4"/>
+      <c r="C25" s="4" t="s">
+        <v>3981</v>
+      </c>
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
       <c r="F25" s="3"/>
@@ -59065,7 +59138,9 @@
       <c r="B26" s="6" t="s">
         <v>3820</v>
       </c>
-      <c r="C26" s="4"/>
+      <c r="C26" s="4" t="s">
+        <v>3924</v>
+      </c>
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
       <c r="F26" s="3"/>

</xml_diff>